<commit_message>
now ready to fill json and more test
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B61224-7F26-4476-A7C2-73BA46D26084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA5EE0B-E302-4826-820B-4663805B6484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">columnas!$A$1:$G$116</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">kwords!$A$1:$E$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">kwords!$A$1:$E$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -918,8 +918,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -973,7 +973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -996,7 +996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>98</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>98</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>98</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>98</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>98</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>98</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>98</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>98</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>98</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>98</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>98</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>98</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>98</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>98</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>98</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>98</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>98</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>98</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>98</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>98</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>98</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>97</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>97</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>97</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>97</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>97</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>97</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>97</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>97</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>97</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>97</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>97</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>97</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>97</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>97</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>97</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>97</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>97</v>
       </c>
@@ -3599,12 +3599,7 @@
   <autoFilter ref="A1:G116" xr:uid="{30924B49-0232-4E80-8796-B64087399799}">
     <filterColumn colId="0">
       <filters>
-        <filter val="agencia"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Bs00"/>
+        <filter val="distribuidora"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3619,7 +3614,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3777,7 +3772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -3791,10 +3786,10 @@
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -3811,7 +3806,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -3828,7 +3823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -3845,7 +3840,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -3862,7 +3857,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -3879,7 +3874,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -3896,7 +3891,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -3913,7 +3908,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -3930,7 +3925,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>98</v>
       </c>
@@ -3947,7 +3942,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -3964,7 +3959,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -3981,7 +3976,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -3998,7 +3993,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -4015,7 +4010,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -4032,7 +4027,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -4049,7 +4044,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -4066,7 +4061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -4185,7 +4180,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -4202,7 +4197,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>98</v>
       </c>
@@ -4219,7 +4214,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -4236,7 +4231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -4253,7 +4248,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -4270,7 +4265,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -4287,7 +4282,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>98</v>
       </c>
@@ -4304,7 +4299,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -4321,7 +4316,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -4338,7 +4333,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -4355,7 +4350,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -4372,7 +4367,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -4390,10 +4385,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E35" xr:uid="{E179BDF2-7707-4A54-9B49-BD9D3898BE0C}">
-    <filterColumn colId="1">
+  <autoFilter ref="A1:E45" xr:uid="{E179BDF2-7707-4A54-9B49-BD9D3898BE0C}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Bs"/>
+        <filter val="distribuidora"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
to present in monday
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA5EE0B-E302-4826-820B-4663805B6484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32B4FA6-4944-4E95-B42A-5E7EF026AE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="kwords" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">columnas!$A$1:$G$116</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">kwords!$A$1:$E$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">columnas!$A$1:$G$147</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">kwords!$A$1:$E$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="141">
   <si>
     <t>fechaInicial</t>
   </si>
@@ -396,6 +396,75 @@
   </si>
   <si>
     <t>Bs00</t>
+  </si>
+  <si>
+    <t>Nro APP</t>
+  </si>
+  <si>
+    <t>Cierre de cobrador</t>
+  </si>
+  <si>
+    <t>recibo de caja</t>
+  </si>
+  <si>
+    <t>Fecha Recibo</t>
+  </si>
+  <si>
+    <t>Cod Cliente</t>
+  </si>
+  <si>
+    <t>Nombre cliente</t>
+  </si>
+  <si>
+    <t>fechaCheque</t>
+  </si>
+  <si>
+    <t>Nro Cheque</t>
+  </si>
+  <si>
+    <t>Banco Cheque</t>
+  </si>
+  <si>
+    <t>EqBs</t>
+  </si>
+  <si>
+    <t>Us</t>
+  </si>
+  <si>
+    <t>Cheque</t>
+  </si>
+  <si>
+    <t>transferencia</t>
+  </si>
+  <si>
+    <t>recibo de cobranza</t>
+  </si>
+  <si>
+    <t>Total Cobrado:</t>
+  </si>
+  <si>
+    <t>Nº de APP</t>
+  </si>
+  <si>
+    <t>banco</t>
+  </si>
+  <si>
+    <t>recepcion en caja</t>
+  </si>
+  <si>
+    <t>Recepción en caja</t>
+  </si>
+  <si>
+    <t>Total efectivo recibido</t>
+  </si>
+  <si>
+    <t>Fecha Transferencia</t>
+  </si>
+  <si>
+    <t>Banco Transferencia</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -716,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A1:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>44966</v>
+        <v>44972</v>
       </c>
       <c r="F2" t="s">
         <v>87</v>
@@ -784,7 +853,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G4" t="s">
         <v>65</v>
@@ -798,7 +867,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G5" t="s">
         <v>67</v>
@@ -812,7 +881,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G6" t="s">
         <v>69</v>
@@ -826,7 +895,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>
@@ -840,7 +909,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G8" t="s">
         <v>73</v>
@@ -854,7 +923,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G9" t="s">
         <v>75</v>
@@ -868,7 +937,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G10" t="s">
         <v>77</v>
@@ -882,7 +951,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G11" t="s">
         <v>79</v>
@@ -896,7 +965,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G12" t="s">
         <v>81</v>
@@ -916,10 +985,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30924B49-0232-4E80-8796-B64087399799}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -1387,7 +1456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -1410,7 +1479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -1433,7 +1502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -1456,7 +1525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1479,7 +1548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -1502,7 +1571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -1525,7 +1594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -1548,7 +1617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -1571,7 +1640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -1594,7 +1663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -1617,7 +1686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -1640,7 +1709,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -1663,7 +1732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -3158,7 +3227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -3181,7 +3250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -3204,7 +3273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>97</v>
       </c>
@@ -3227,7 +3296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>97</v>
       </c>
@@ -3250,7 +3319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>97</v>
       </c>
@@ -3273,7 +3342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>97</v>
       </c>
@@ -3296,7 +3365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>97</v>
       </c>
@@ -3319,7 +3388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>97</v>
       </c>
@@ -3342,7 +3411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>97</v>
       </c>
@@ -3365,7 +3434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>97</v>
       </c>
@@ -3388,7 +3457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>97</v>
       </c>
@@ -3411,7 +3480,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>97</v>
       </c>
@@ -3434,7 +3503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>97</v>
       </c>
@@ -3457,7 +3526,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>97</v>
       </c>
@@ -3480,7 +3549,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>97</v>
       </c>
@@ -3503,7 +3572,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>97</v>
       </c>
@@ -3526,7 +3595,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>97</v>
       </c>
@@ -3549,7 +3618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>97</v>
       </c>
@@ -3572,7 +3641,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>97</v>
       </c>
@@ -3595,11 +3664,734 @@
         <v>23</v>
       </c>
     </row>
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>97</v>
+      </c>
+      <c r="B117" t="s">
+        <v>119</v>
+      </c>
+      <c r="C117" t="s">
+        <v>30</v>
+      </c>
+      <c r="D117" t="s">
+        <v>120</v>
+      </c>
+      <c r="E117" t="s">
+        <v>120</v>
+      </c>
+      <c r="F117" t="s">
+        <v>118</v>
+      </c>
+      <c r="G117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>97</v>
+      </c>
+      <c r="B118" t="s">
+        <v>119</v>
+      </c>
+      <c r="C118" t="s">
+        <v>30</v>
+      </c>
+      <c r="D118" t="s">
+        <v>120</v>
+      </c>
+      <c r="E118" t="s">
+        <v>120</v>
+      </c>
+      <c r="F118" t="s">
+        <v>121</v>
+      </c>
+      <c r="G118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>97</v>
+      </c>
+      <c r="B119" t="s">
+        <v>119</v>
+      </c>
+      <c r="C119" t="s">
+        <v>30</v>
+      </c>
+      <c r="D119" t="s">
+        <v>120</v>
+      </c>
+      <c r="E119" t="s">
+        <v>120</v>
+      </c>
+      <c r="F119" t="s">
+        <v>122</v>
+      </c>
+      <c r="G119">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>97</v>
+      </c>
+      <c r="B120" t="s">
+        <v>119</v>
+      </c>
+      <c r="C120" t="s">
+        <v>30</v>
+      </c>
+      <c r="D120" t="s">
+        <v>120</v>
+      </c>
+      <c r="E120" t="s">
+        <v>120</v>
+      </c>
+      <c r="F120" t="s">
+        <v>123</v>
+      </c>
+      <c r="G120">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>97</v>
+      </c>
+      <c r="B121" t="s">
+        <v>119</v>
+      </c>
+      <c r="C121" t="s">
+        <v>5</v>
+      </c>
+      <c r="D121" t="s">
+        <v>54</v>
+      </c>
+      <c r="E121" t="s">
+        <v>120</v>
+      </c>
+      <c r="F121" t="s">
+        <v>5</v>
+      </c>
+      <c r="G121">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>97</v>
+      </c>
+      <c r="B122" t="s">
+        <v>119</v>
+      </c>
+      <c r="C122" t="s">
+        <v>128</v>
+      </c>
+      <c r="D122" t="s">
+        <v>54</v>
+      </c>
+      <c r="E122" t="s">
+        <v>120</v>
+      </c>
+      <c r="F122" t="s">
+        <v>128</v>
+      </c>
+      <c r="G122">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>97</v>
+      </c>
+      <c r="B123" t="s">
+        <v>119</v>
+      </c>
+      <c r="C123" t="s">
+        <v>30</v>
+      </c>
+      <c r="D123" t="s">
+        <v>129</v>
+      </c>
+      <c r="E123" t="s">
+        <v>120</v>
+      </c>
+      <c r="F123" t="s">
+        <v>124</v>
+      </c>
+      <c r="G123">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>97</v>
+      </c>
+      <c r="B124" t="s">
+        <v>119</v>
+      </c>
+      <c r="C124" t="s">
+        <v>30</v>
+      </c>
+      <c r="D124" t="s">
+        <v>129</v>
+      </c>
+      <c r="E124" t="s">
+        <v>120</v>
+      </c>
+      <c r="F124" t="s">
+        <v>125</v>
+      </c>
+      <c r="G124">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>97</v>
+      </c>
+      <c r="B125" t="s">
+        <v>119</v>
+      </c>
+      <c r="C125" t="s">
+        <v>30</v>
+      </c>
+      <c r="D125" t="s">
+        <v>129</v>
+      </c>
+      <c r="E125" t="s">
+        <v>120</v>
+      </c>
+      <c r="F125" t="s">
+        <v>126</v>
+      </c>
+      <c r="G125">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>97</v>
+      </c>
+      <c r="B126" t="s">
+        <v>119</v>
+      </c>
+      <c r="C126" t="s">
+        <v>5</v>
+      </c>
+      <c r="D126" t="s">
+        <v>129</v>
+      </c>
+      <c r="E126" t="s">
+        <v>120</v>
+      </c>
+      <c r="F126" t="s">
+        <v>5</v>
+      </c>
+      <c r="G126">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>97</v>
+      </c>
+      <c r="B127" t="s">
+        <v>119</v>
+      </c>
+      <c r="C127" t="s">
+        <v>128</v>
+      </c>
+      <c r="D127" t="s">
+        <v>129</v>
+      </c>
+      <c r="E127" t="s">
+        <v>120</v>
+      </c>
+      <c r="F127" t="s">
+        <v>128</v>
+      </c>
+      <c r="G127">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>97</v>
+      </c>
+      <c r="B128" t="s">
+        <v>119</v>
+      </c>
+      <c r="C128" t="s">
+        <v>30</v>
+      </c>
+      <c r="D128" t="s">
+        <v>130</v>
+      </c>
+      <c r="E128" t="s">
+        <v>120</v>
+      </c>
+      <c r="F128" t="s">
+        <v>138</v>
+      </c>
+      <c r="G128">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>97</v>
+      </c>
+      <c r="B129" t="s">
+        <v>119</v>
+      </c>
+      <c r="C129" t="s">
+        <v>30</v>
+      </c>
+      <c r="D129" t="s">
+        <v>130</v>
+      </c>
+      <c r="E129" t="s">
+        <v>120</v>
+      </c>
+      <c r="F129" t="s">
+        <v>139</v>
+      </c>
+      <c r="G129">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>97</v>
+      </c>
+      <c r="B130" t="s">
+        <v>119</v>
+      </c>
+      <c r="C130" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" t="s">
+        <v>130</v>
+      </c>
+      <c r="E130" t="s">
+        <v>120</v>
+      </c>
+      <c r="F130" t="s">
+        <v>5</v>
+      </c>
+      <c r="G130">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>97</v>
+      </c>
+      <c r="B131" t="s">
+        <v>119</v>
+      </c>
+      <c r="C131" t="s">
+        <v>128</v>
+      </c>
+      <c r="D131" t="s">
+        <v>130</v>
+      </c>
+      <c r="E131" t="s">
+        <v>120</v>
+      </c>
+      <c r="F131" t="s">
+        <v>128</v>
+      </c>
+      <c r="G131">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>97</v>
+      </c>
+      <c r="B132" t="s">
+        <v>119</v>
+      </c>
+      <c r="C132" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132" t="s">
+        <v>12</v>
+      </c>
+      <c r="E132" t="s">
+        <v>120</v>
+      </c>
+      <c r="F132" t="s">
+        <v>5</v>
+      </c>
+      <c r="G132">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>97</v>
+      </c>
+      <c r="B133" t="s">
+        <v>119</v>
+      </c>
+      <c r="C133" t="s">
+        <v>128</v>
+      </c>
+      <c r="D133" t="s">
+        <v>12</v>
+      </c>
+      <c r="E133" t="s">
+        <v>120</v>
+      </c>
+      <c r="F133" t="s">
+        <v>128</v>
+      </c>
+      <c r="G133">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>97</v>
+      </c>
+      <c r="B134" t="s">
+        <v>119</v>
+      </c>
+      <c r="C134" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" t="s">
+        <v>12</v>
+      </c>
+      <c r="E134" t="s">
+        <v>120</v>
+      </c>
+      <c r="F134" t="s">
+        <v>127</v>
+      </c>
+      <c r="G134">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>97</v>
+      </c>
+      <c r="B135" t="s">
+        <v>119</v>
+      </c>
+      <c r="C135" t="s">
+        <v>5</v>
+      </c>
+      <c r="D135" t="s">
+        <v>11</v>
+      </c>
+      <c r="E135" t="s">
+        <v>120</v>
+      </c>
+      <c r="F135" t="s">
+        <v>5</v>
+      </c>
+      <c r="G135">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>97</v>
+      </c>
+      <c r="B136" t="s">
+        <v>119</v>
+      </c>
+      <c r="C136" t="s">
+        <v>5</v>
+      </c>
+      <c r="D136" t="s">
+        <v>54</v>
+      </c>
+      <c r="E136" t="s">
+        <v>135</v>
+      </c>
+      <c r="F136" t="s">
+        <v>5</v>
+      </c>
+      <c r="G136">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>97</v>
+      </c>
+      <c r="B137" t="s">
+        <v>119</v>
+      </c>
+      <c r="C137" t="s">
+        <v>128</v>
+      </c>
+      <c r="D137" t="s">
+        <v>54</v>
+      </c>
+      <c r="E137" t="s">
+        <v>135</v>
+      </c>
+      <c r="F137" t="s">
+        <v>128</v>
+      </c>
+      <c r="G137">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>97</v>
+      </c>
+      <c r="B138" t="s">
+        <v>119</v>
+      </c>
+      <c r="C138" t="s">
+        <v>5</v>
+      </c>
+      <c r="D138" t="s">
+        <v>54</v>
+      </c>
+      <c r="E138" t="s">
+        <v>135</v>
+      </c>
+      <c r="F138" t="s">
+        <v>127</v>
+      </c>
+      <c r="G138">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>97</v>
+      </c>
+      <c r="B139" t="s">
+        <v>119</v>
+      </c>
+      <c r="C139" t="s">
+        <v>5</v>
+      </c>
+      <c r="D139" t="s">
+        <v>129</v>
+      </c>
+      <c r="E139" t="s">
+        <v>135</v>
+      </c>
+      <c r="F139" t="s">
+        <v>5</v>
+      </c>
+      <c r="G139">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>97</v>
+      </c>
+      <c r="B140" t="s">
+        <v>119</v>
+      </c>
+      <c r="C140" t="s">
+        <v>5</v>
+      </c>
+      <c r="D140" t="s">
+        <v>129</v>
+      </c>
+      <c r="E140" t="s">
+        <v>135</v>
+      </c>
+      <c r="F140" t="s">
+        <v>128</v>
+      </c>
+      <c r="G140">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>97</v>
+      </c>
+      <c r="B141" t="s">
+        <v>119</v>
+      </c>
+      <c r="C141" t="s">
+        <v>5</v>
+      </c>
+      <c r="D141" t="s">
+        <v>129</v>
+      </c>
+      <c r="E141" t="s">
+        <v>135</v>
+      </c>
+      <c r="F141" t="s">
+        <v>127</v>
+      </c>
+      <c r="G141">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>97</v>
+      </c>
+      <c r="B142" t="s">
+        <v>119</v>
+      </c>
+      <c r="C142" t="s">
+        <v>30</v>
+      </c>
+      <c r="D142" t="s">
+        <v>130</v>
+      </c>
+      <c r="E142" t="s">
+        <v>135</v>
+      </c>
+      <c r="F142" t="s">
+        <v>138</v>
+      </c>
+      <c r="G142">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>97</v>
+      </c>
+      <c r="B143" t="s">
+        <v>119</v>
+      </c>
+      <c r="C143" t="s">
+        <v>30</v>
+      </c>
+      <c r="D143" t="s">
+        <v>130</v>
+      </c>
+      <c r="E143" t="s">
+        <v>135</v>
+      </c>
+      <c r="F143" t="s">
+        <v>134</v>
+      </c>
+      <c r="G143">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>97</v>
+      </c>
+      <c r="B144" t="s">
+        <v>119</v>
+      </c>
+      <c r="C144" t="s">
+        <v>5</v>
+      </c>
+      <c r="D144" t="s">
+        <v>130</v>
+      </c>
+      <c r="E144" t="s">
+        <v>135</v>
+      </c>
+      <c r="F144" t="s">
+        <v>5</v>
+      </c>
+      <c r="G144">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>97</v>
+      </c>
+      <c r="B145" t="s">
+        <v>119</v>
+      </c>
+      <c r="C145" t="s">
+        <v>5</v>
+      </c>
+      <c r="D145" t="s">
+        <v>130</v>
+      </c>
+      <c r="E145" t="s">
+        <v>135</v>
+      </c>
+      <c r="F145" t="s">
+        <v>128</v>
+      </c>
+      <c r="G145">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>97</v>
+      </c>
+      <c r="B146" t="s">
+        <v>119</v>
+      </c>
+      <c r="C146" t="s">
+        <v>5</v>
+      </c>
+      <c r="D146" t="s">
+        <v>130</v>
+      </c>
+      <c r="E146" t="s">
+        <v>135</v>
+      </c>
+      <c r="F146" t="s">
+        <v>127</v>
+      </c>
+      <c r="G146">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>97</v>
+      </c>
+      <c r="B147" t="s">
+        <v>119</v>
+      </c>
+      <c r="C147" t="s">
+        <v>5</v>
+      </c>
+      <c r="D147" t="s">
+        <v>11</v>
+      </c>
+      <c r="E147" t="s">
+        <v>135</v>
+      </c>
+      <c r="F147" t="s">
+        <v>5</v>
+      </c>
+      <c r="G147">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G116" xr:uid="{30924B49-0232-4E80-8796-B64087399799}">
+  <autoFilter ref="A1:G147" xr:uid="{30924B49-0232-4E80-8796-B64087399799}">
     <filterColumn colId="0">
       <filters>
         <filter val="distribuidora"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Detalle Operaciones"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Bs"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3611,10 +4403,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E179BDF2-7707-4A54-9B49-BD9D3898BE0C}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3772,7 +4564,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -3789,7 +4581,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -3806,7 +4598,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -3823,7 +4615,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -3840,7 +4632,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -3857,7 +4649,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -3874,7 +4666,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -3891,7 +4683,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -4384,11 +5176,84 @@
         <v>102</v>
       </c>
     </row>
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E45" xr:uid="{E179BDF2-7707-4A54-9B49-BD9D3898BE0C}">
+  <autoFilter ref="A1:E49" xr:uid="{E179BDF2-7707-4A54-9B49-BD9D3898BE0C}">
     <filterColumn colId="0">
       <filters>
         <filter val="distribuidora"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Bs"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
box closing scrap finished
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32B4FA6-4944-4E95-B42A-5E7EF026AE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D31915C-EC45-44A4-B912-420EE86D5192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -785,9 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:I13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -987,8 +985,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,7 +1431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -1456,7 +1454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -1479,7 +1477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -1502,7 +1500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -1525,7 +1523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1548,7 +1546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -1571,7 +1569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -1594,7 +1592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -1617,7 +1615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -1640,7 +1638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -1663,7 +1661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -1686,7 +1684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -1709,7 +1707,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -1732,7 +1730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -3227,7 +3225,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -3250,7 +3248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -3273,7 +3271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>97</v>
       </c>
@@ -3296,7 +3294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>97</v>
       </c>
@@ -3319,7 +3317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>97</v>
       </c>
@@ -3342,7 +3340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>97</v>
       </c>
@@ -3365,7 +3363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>97</v>
       </c>
@@ -3388,7 +3386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>97</v>
       </c>
@@ -3411,7 +3409,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>97</v>
       </c>
@@ -3434,7 +3432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>97</v>
       </c>
@@ -3457,7 +3455,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>97</v>
       </c>
@@ -3480,7 +3478,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>97</v>
       </c>
@@ -3503,7 +3501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>97</v>
       </c>
@@ -3526,7 +3524,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>97</v>
       </c>
@@ -3549,7 +3547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>97</v>
       </c>
@@ -3572,7 +3570,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>97</v>
       </c>
@@ -3595,7 +3593,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>97</v>
       </c>
@@ -3618,7 +3616,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>97</v>
       </c>
@@ -3641,7 +3639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>97</v>
       </c>
@@ -3664,7 +3662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>97</v>
       </c>
@@ -3687,7 +3685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>97</v>
       </c>
@@ -3710,7 +3708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>97</v>
       </c>
@@ -3733,7 +3731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>97</v>
       </c>
@@ -3756,7 +3754,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>97</v>
       </c>
@@ -3779,7 +3777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>97</v>
       </c>
@@ -3802,7 +3800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>97</v>
       </c>
@@ -3825,7 +3823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>97</v>
       </c>
@@ -3848,7 +3846,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>97</v>
       </c>
@@ -3871,7 +3869,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>97</v>
       </c>
@@ -3894,7 +3892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>97</v>
       </c>
@@ -3917,7 +3915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>97</v>
       </c>
@@ -3940,7 +3938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>97</v>
       </c>
@@ -3963,7 +3961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>97</v>
       </c>
@@ -3986,7 +3984,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>97</v>
       </c>
@@ -4009,7 +4007,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>97</v>
       </c>
@@ -4032,7 +4030,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>97</v>
       </c>
@@ -4055,7 +4053,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>97</v>
       </c>
@@ -4078,7 +4076,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>97</v>
       </c>
@@ -4101,7 +4099,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>97</v>
       </c>
@@ -4124,7 +4122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>97</v>
       </c>
@@ -4147,7 +4145,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>97</v>
       </c>
@@ -4170,7 +4168,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>97</v>
       </c>
@@ -4193,7 +4191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>97</v>
       </c>
@@ -4201,7 +4199,7 @@
         <v>119</v>
       </c>
       <c r="C140" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="D140" t="s">
         <v>129</v>
@@ -4216,7 +4214,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>97</v>
       </c>
@@ -4239,7 +4237,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>97</v>
       </c>
@@ -4262,7 +4260,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>97</v>
       </c>
@@ -4285,7 +4283,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>97</v>
       </c>
@@ -4308,7 +4306,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>97</v>
       </c>
@@ -4316,7 +4314,7 @@
         <v>119</v>
       </c>
       <c r="C145" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="D145" t="s">
         <v>130</v>
@@ -4331,7 +4329,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>97</v>
       </c>
@@ -4354,7 +4352,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>97</v>
       </c>
@@ -4382,16 +4380,6 @@
     <filterColumn colId="0">
       <filters>
         <filter val="distribuidora"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Detalle Operaciones"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Bs"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4405,8 +4393,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4564,7 +4552,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -4581,7 +4569,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -4598,7 +4586,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -4615,7 +4603,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -4632,7 +4620,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -4649,7 +4637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -4666,7 +4654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -4683,7 +4671,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -5176,7 +5164,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -5193,7 +5181,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -5210,7 +5198,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -5227,7 +5215,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -5251,11 +5239,6 @@
         <filter val="distribuidora"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Bs"/>
-      </filters>
-    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
with sgv data in csv ccaj details
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC3DBFF-A818-4F13-BC25-D7D50CD4B335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917B2CAB-C3FD-413B-97B9-ED0889045917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
     <t>NO</t>
   </si>
   <si>
-    <t>PROCESAR</t>
+    <t>COMPLETO</t>
   </si>
 </sst>
 </file>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,10 +873,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>45013</v>
+        <v>45016</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="G2" t="s">
         <v>60</v>
@@ -899,7 +899,7 @@
         <v>45016</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="G3" t="s">
         <v>63</v>
@@ -959,7 +959,7 @@
         <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="F6" t="s">
         <v>154</v>
@@ -996,7 +996,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>154</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
         <v>73</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="G12" t="s">
         <v>81</v>
@@ -1105,7 +1105,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
almost finish with tutorial
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521A303C-99D5-483D-BED6-377FFEBCA51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370F5677-D231-4CF3-AA85-7383201ED80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="20190" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="167">
   <si>
     <t>fechaInicial</t>
   </si>
@@ -537,14 +537,20 @@
     <t>NO</t>
   </si>
   <si>
-    <t>PROCESAR</t>
+    <t>PARA EL SGV</t>
+  </si>
+  <si>
+    <t>DATOS PARA EL SAP</t>
+  </si>
+  <si>
+    <t>COMPLETO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,8 +572,16 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,8 +594,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -634,11 +654,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -650,6 +679,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -947,19 +984,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F1" t="s">
+      <c r="A1" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="F1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="10" t="s">
         <v>142</v>
       </c>
     </row>
@@ -970,7 +1011,7 @@
       <c r="B2" s="1">
         <v>45035</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>87</v>
       </c>
       <c r="G2" t="s">
@@ -993,7 +1034,7 @@
       <c r="B3" s="1">
         <v>45035</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="9" t="s">
         <v>87</v>
       </c>
       <c r="G3" t="s">
@@ -1010,7 +1051,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G4" t="s">
@@ -1031,9 +1072,9 @@
         <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G5" t="s">
@@ -1054,9 +1095,9 @@
         <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G6" t="s">
@@ -1073,7 +1114,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+      <c r="F7" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G7" t="s">
@@ -1090,7 +1131,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
+      <c r="F8" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G8" t="s">
@@ -1107,7 +1148,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
+      <c r="F9" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G9" t="s">
@@ -1124,7 +1165,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+      <c r="F10" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G10" t="s">
@@ -1141,7 +1182,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+      <c r="F11" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G11" t="s">
@@ -1158,7 +1199,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+      <c r="F12" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G12" t="s">
@@ -1175,6 +1216,10 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="12"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1218,6 +1263,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A15:B15"/>
+  </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{6E3AC62A-2010-4956-85C8-7844790103A0}">
       <formula1>"COMPLETO,DESCARGAR,PROCESAR"</formula1>
@@ -4645,11 +4694,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E179BDF2-7707-4A54-9B49-BD9D3898BE0C}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4943,7 +4991,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -4960,7 +5008,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>98</v>
       </c>
@@ -4977,7 +5025,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -4994,7 +5042,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -5011,7 +5059,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -5028,7 +5076,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -5045,7 +5093,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -5062,7 +5110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -5079,7 +5127,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -5096,7 +5144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -5113,7 +5161,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>98</v>
       </c>
@@ -5130,7 +5178,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>98</v>
       </c>
@@ -5147,7 +5195,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>98</v>
       </c>
@@ -5164,7 +5212,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -5181,7 +5229,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -5198,7 +5246,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -5215,7 +5263,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -5232,7 +5280,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>98</v>
       </c>
@@ -5249,7 +5297,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -5266,7 +5314,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -5283,7 +5331,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -5300,7 +5348,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -5317,7 +5365,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>98</v>
       </c>
@@ -5334,7 +5382,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -5351,7 +5399,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -5368,7 +5416,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -5385,7 +5433,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -5402,7 +5450,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -5488,13 +5536,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E49" xr:uid="{E179BDF2-7707-4A54-9B49-BD9D3898BE0C}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="distribuidora"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E49" xr:uid="{E179BDF2-7707-4A54-9B49-BD9D3898BE0C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
paths for currency type fixed
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE94D59B-E8C0-4BBC-9999-08351EF97F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF57BAAB-A96C-449C-8EF2-0B63B70F8925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="225" yWindow="150" windowWidth="20265" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -969,7 +969,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1009,7 @@
         <v>45061</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="G2" t="s">
         <v>60</v>
@@ -1032,7 +1032,7 @@
         <v>45064</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="G3" t="s">
         <v>63</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F7" s="9" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
fix large paths 2
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF57BAAB-A96C-449C-8EF2-0B63B70F8925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D586EAB-E147-4F9B-BBC6-092DEF79D42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="225" yWindow="150" windowWidth="20265" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -969,7 +969,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,10 +1006,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>45061</v>
+        <v>45064</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
         <v>60</v>
@@ -1032,7 +1032,7 @@
         <v>45064</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
         <v>63</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F7" s="9" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
ouput and sapinfo added
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/bot4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{182AD21A-ADA4-4193-AF47-CA757E386196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68F6B220-3D7B-4DC1-803C-581D02133103}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEEFE8C-5C1A-463A-AEC9-EB88E120E219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
     <t>NO</t>
   </si>
   <si>
-    <t>DESCARGAR</t>
+    <t>COMPLETO</t>
   </si>
 </sst>
 </file>
@@ -969,7 +969,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
remove file in sapinfo
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/bot4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEEFE8C-5C1A-463A-AEC9-EB88E120E219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{6EEEFE8C-5C1A-463A-AEC9-EB88E120E219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA606A15-B169-49F5-8E31-330D08F0BF22}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
     <t>NO</t>
   </si>
   <si>
-    <t>COMPLETO</t>
+    <t>PROCESAR</t>
   </si>
 </sst>
 </file>
@@ -969,7 +969,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1009,7 @@
         <v>45078</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
         <v>60</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F12" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G12" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
empty ditc in get_matrix fix
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7DD058-D46B-4315-A160-3F9788C831FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23285B0E-B53A-482D-BD0A-88A38B998274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="150" windowWidth="20265" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="165">
   <si>
     <t>fechaInicial</t>
   </si>
@@ -537,10 +537,7 @@
     <t>PRD HANA</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>COMPLETO</t>
+    <t>PROCESAR</t>
   </si>
 </sst>
 </file>
@@ -969,7 +966,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>45131</v>
+        <v>45124</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>87</v>
@@ -1032,7 +1029,7 @@
         <v>45131</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
         <v>63</v>
@@ -1049,7 +1046,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F4" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
         <v>65</v>
@@ -1069,10 +1066,10 @@
         <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
         <v>67</v>
@@ -1089,7 +1086,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F6" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
         <v>69</v>
@@ -1106,7 +1103,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F7" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>
@@ -1123,7 +1120,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
         <v>73</v>
@@ -1140,7 +1137,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F9" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
         <v>75</v>
@@ -1157,7 +1154,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F10" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
         <v>77</v>
@@ -1174,7 +1171,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F11" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
         <v>79</v>
@@ -1191,7 +1188,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F12" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
tries in reading files
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23285B0E-B53A-482D-BD0A-88A38B998274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8514FE-3712-4BF5-8EB3-0796DAE724A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="166">
   <si>
     <t>fechaInicial</t>
   </si>
@@ -537,7 +537,10 @@
     <t>PRD HANA</t>
   </si>
   <si>
-    <t>PROCESAR</t>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>COMPLETO</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1006,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>45124</v>
+        <v>45138</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G2" t="s">
         <v>60</v>
@@ -1026,10 +1029,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>45131</v>
+        <v>45138</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G3" t="s">
         <v>63</v>
@@ -1046,7 +1049,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F4" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G4" t="s">
         <v>65</v>
@@ -1066,7 +1069,7 @@
         <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>87</v>
@@ -1086,7 +1089,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F6" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G6" t="s">
         <v>69</v>
@@ -1103,7 +1106,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F7" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>
@@ -1120,7 +1123,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G8" t="s">
         <v>73</v>
@@ -1137,7 +1140,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F9" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G9" t="s">
         <v>75</v>
@@ -1154,7 +1157,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F10" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G10" t="s">
         <v>77</v>
@@ -1171,7 +1174,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F11" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G11" t="s">
         <v>79</v>
@@ -1188,7 +1191,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F12" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G12" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
click page to update page and validate in get_matrix
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\bot4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8514FE-3712-4BF5-8EB3-0796DAE724A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570EB7F1-263D-40E6-8E38-69AF1180E21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="150" windowWidth="20265" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
     <t>NO</t>
   </si>
   <si>
-    <t>COMPLETO</t>
+    <t>PROCESAR</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>45138</v>
+        <v>45143</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>164</v>
@@ -1072,7 +1072,7 @@
         <v>165</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="G5" t="s">
         <v>67</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F6" s="9" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
         <v>69</v>

</xml_diff>